<commit_message>
Updated with WiP design for main control board
* based off BBB power cape
* using sparkfun libraries
* includes necessary sparkfun libraries
</commit_message>
<xml_diff>
--- a/design/powerBoM.xlsx
+++ b/design/powerBoM.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\William\OneDrive\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="516" yWindow="624" windowWidth="15996" windowHeight="5244"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162912" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="145621" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Price</t>
   </si>
@@ -88,6 +83,9 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/TE-Connectivity-Raychem/RUEF500-2/?qs=sGAEpiMZZMsgjL4JkW1EEVNr4NcEMyYykh5e2ljN8mo%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Maxim-Integrated/MAX16907SAUE-V+/?qs=sGAEpiMZZMtitjHzVIkrqcnFxyrtXyRUF09tT8a55%252bo%3d</t>
   </si>
 </sst>
 </file>
@@ -439,7 +437,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -450,28 +448,28 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="4" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="C1" s="1"/>
       <c r="E1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="27.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -497,7 +495,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -523,7 +521,7 @@
         <v>59.11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -536,8 +534,11 @@
       <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -550,8 +551,11 @@
       <c r="D6" s="4">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E6" s="1">
+        <v>6.26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -565,7 +569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -593,7 +597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>19</v>
       </c>
@@ -609,7 +613,7 @@
       <c r="E12" s="9"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
@@ -623,7 +627,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" ht="15" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
     </row>
   </sheetData>
@@ -644,7 +648,9 @@
     <hyperlink ref="B12" r:id="rId14"/>
     <hyperlink ref="C12" r:id="rId15"/>
     <hyperlink ref="D12" r:id="rId16"/>
+    <hyperlink ref="E5" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated power BoM with sourced components.
</commit_message>
<xml_diff>
--- a/design/powerBoM.xlsx
+++ b/design/powerBoM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Price</t>
   </si>
@@ -86,6 +86,24 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/Maxim-Integrated/MAX16907SAUE-V+/?qs=sGAEpiMZZMtitjHzVIkrqcnFxyrtXyRUF09tT8a55%252bo%3d</t>
+  </si>
+  <si>
+    <t>ACTUALLY BOUGHT:</t>
+  </si>
+  <si>
+    <t>12V DC/DC Converter</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Power-Sonic/PS-12120F2/?qs=sGAEpiMZZMuXcNZ31nzYhWCg8Aa0ccFGvNDs0yXFGmM%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Mean-Well/RSD-100B-12/?qs=sGAEpiMZZMvGsmoEFRKS8P9bZCysYvvSGN8daVBtngg%3d</t>
+  </si>
+  <si>
+    <t>Wire</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Alpha-Wire/6459-OR005/?qs=sGAEpiMZZMv1%2f%252b2kKkGMBdDOvp5WNg%252btn9IFOpL1GP0%3d</t>
   </si>
 </sst>
 </file>
@@ -141,7 +159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -164,6 +182,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -437,7 +462,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -445,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,8 +652,36 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="17" spans="3:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="C17" s="1"/>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -649,8 +702,12 @@
     <hyperlink ref="C12" r:id="rId15"/>
     <hyperlink ref="D12" r:id="rId16"/>
     <hyperlink ref="E5" r:id="rId17"/>
+    <hyperlink ref="C18" r:id="rId18"/>
+    <hyperlink ref="B18" r:id="rId19"/>
+    <hyperlink ref="D18" r:id="rId20"/>
+    <hyperlink ref="D19" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>